<commit_message>
File change commit //ignore
</commit_message>
<xml_diff>
--- a/web/src/main/resources/public/name_entry_template.xlsx
+++ b/web/src/main/resources/public/name_entry_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="584" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="991" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,21 +15,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Tone</t>
-  </si>
-  <si>
     <t>Meaning</t>
   </si>
   <si>
+    <t>Extra information</t>
+  </si>
+  <si>
+    <t>Syllable</t>
+  </si>
+  <si>
+    <t>IPA pronunciation</t>
+  </si>
+  <si>
+    <t>American pronunciation</t>
+  </si>
+  <si>
     <t>Morphology</t>
   </si>
   <si>
-    <t>Location</t>
+    <t>Etymology</t>
+  </si>
+  <si>
+    <t>Variant</t>
+  </si>
+  <si>
+    <t>Media link</t>
+  </si>
+  <si>
+    <t>Personalities</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>Religious</t>
+  </si>
+  <si>
+    <t>Social</t>
+  </si>
+  <si>
+    <t>Geographic</t>
+  </si>
+  <si>
+    <t>Geolocation</t>
   </si>
 </sst>
 </file>
@@ -39,7 +75,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -69,13 +105,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -147,13 +176,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -164,15 +193,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -276,19 +301,19 @@
   <dimension ref="1:340"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="28"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.53441295546559"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2267206477733"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5951417004049"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="8.53441295546559"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="27.9948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.53061224489796"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.219387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.5969387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="8.53061224489796"/>
     <col collapsed="false" hidden="true" max="9" min="8" style="0" width="0"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.1255060728745"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.53441295546559"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="12.1326530612245"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.53061224489796"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -298,7 +323,7 @@
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -307,1024 +332,1060 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5"/>
+      <c r="A2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6"/>
+      <c r="A3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5"/>
+      <c r="A4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
+      <c r="A5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7"/>
+      <c r="A6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7"/>
+      <c r="A7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7"/>
+      <c r="A8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7"/>
+      <c r="A9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7"/>
+      <c r="A10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="7"/>
+      <c r="A11" s="6"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="7"/>
+      <c r="A12" s="6"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7"/>
+      <c r="A13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="7"/>
+      <c r="A14" s="6"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7"/>
+      <c r="A15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7"/>
+      <c r="A16" s="6"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7"/>
+      <c r="A17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7"/>
+      <c r="A18" s="6"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7"/>
+      <c r="A19" s="6"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7"/>
+      <c r="A20" s="6"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7"/>
+      <c r="A21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7"/>
+      <c r="A22" s="6"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5"/>
+      <c r="A24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8"/>
+      <c r="A25" s="7"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5"/>
+      <c r="A26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5"/>
+      <c r="A27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5"/>
+      <c r="A28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5"/>
+      <c r="A29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5"/>
+      <c r="A30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="9"/>
+      <c r="A31" s="8"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5"/>
+      <c r="A32" s="4"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5"/>
+      <c r="A33" s="4"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5"/>
+      <c r="A34" s="4"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5"/>
+      <c r="A36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5"/>
+      <c r="A37" s="4"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5"/>
+      <c r="A38" s="4"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5"/>
+      <c r="A39" s="4"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5"/>
+      <c r="A40" s="4"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5"/>
+      <c r="A41" s="4"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5"/>
+      <c r="A42" s="4"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5"/>
+      <c r="A44" s="4"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5"/>
+      <c r="A45" s="4"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="5"/>
+      <c r="A46" s="4"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5"/>
+      <c r="A47" s="4"/>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5"/>
+      <c r="A48" s="4"/>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5"/>
+      <c r="A49" s="4"/>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5"/>
+      <c r="A50" s="4"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="5"/>
+      <c r="A51" s="4"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5"/>
+      <c r="A52" s="4"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5"/>
+      <c r="A53" s="4"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5"/>
+      <c r="A54" s="4"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="5"/>
+      <c r="A55" s="4"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5"/>
+      <c r="A57" s="4"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="5"/>
+      <c r="A58" s="4"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="5"/>
+      <c r="A59" s="4"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="5"/>
+      <c r="A60" s="4"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="5"/>
+      <c r="A61" s="4"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="5"/>
+      <c r="A62" s="4"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="8"/>
+      <c r="A63" s="7"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="8"/>
+      <c r="A64" s="7"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="8"/>
+      <c r="A65" s="7"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="8"/>
+      <c r="A66" s="7"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="5"/>
+      <c r="A67" s="4"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="5"/>
+      <c r="A68" s="4"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="9"/>
+      <c r="A69" s="8"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="5"/>
+      <c r="A70" s="4"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="5"/>
+      <c r="A71" s="4"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="5"/>
+      <c r="A73" s="4"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="5"/>
+      <c r="A74" s="4"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="5"/>
+      <c r="A75" s="4"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="5"/>
+      <c r="A76" s="4"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="5"/>
+      <c r="A77" s="4"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="5"/>
+      <c r="A78" s="4"/>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="5"/>
+      <c r="A79" s="4"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="5"/>
+      <c r="A80" s="4"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="5"/>
+      <c r="A82" s="4"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="5"/>
+      <c r="A83" s="4"/>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="5"/>
+      <c r="A84" s="4"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="5"/>
+      <c r="A85" s="4"/>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="5"/>
+      <c r="A86" s="4"/>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="5"/>
+      <c r="A87" s="4"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="5"/>
+      <c r="A88" s="4"/>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0"/>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="5"/>
+      <c r="A90" s="4"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="9"/>
+      <c r="A91" s="8"/>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="5"/>
+      <c r="A92" s="4"/>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0"/>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="5"/>
+      <c r="A94" s="4"/>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="5"/>
+      <c r="A95" s="4"/>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="5"/>
+      <c r="A96" s="4"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="5"/>
+      <c r="A97" s="4"/>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="5"/>
+      <c r="A98" s="4"/>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="5"/>
+      <c r="A99" s="4"/>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="5"/>
+      <c r="A100" s="4"/>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="5"/>
+      <c r="A101" s="4"/>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="5"/>
+      <c r="A102" s="4"/>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="5"/>
+      <c r="A103" s="4"/>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0"/>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="5"/>
+      <c r="A105" s="4"/>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="5"/>
+      <c r="A106" s="4"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="5"/>
+      <c r="A107" s="4"/>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="5"/>
+      <c r="A108" s="4"/>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="5"/>
+      <c r="A109" s="4"/>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="5"/>
+      <c r="A110" s="4"/>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0"/>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="5"/>
+      <c r="A112" s="4"/>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="5"/>
+      <c r="A113" s="4"/>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="5"/>
+      <c r="A114" s="4"/>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="5"/>
+      <c r="A115" s="4"/>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="8"/>
+      <c r="A116" s="7"/>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="5"/>
+      <c r="A117" s="4"/>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="9"/>
+      <c r="A118" s="8"/>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="9"/>
+      <c r="A119" s="8"/>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="9"/>
+      <c r="A120" s="8"/>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="9"/>
+      <c r="A121" s="8"/>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="5"/>
+      <c r="A122" s="4"/>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="5"/>
+      <c r="A123" s="4"/>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="5"/>
+      <c r="A124" s="4"/>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="5"/>
+      <c r="A125" s="4"/>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="5"/>
+      <c r="A126" s="4"/>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0"/>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="5"/>
+      <c r="A128" s="4"/>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="5"/>
+      <c r="A129" s="4"/>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="5"/>
+      <c r="A130" s="4"/>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="5"/>
+      <c r="A131" s="4"/>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="5"/>
+      <c r="A132" s="4"/>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="5"/>
+      <c r="A133" s="4"/>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="5"/>
+      <c r="A134" s="4"/>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0"/>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="5"/>
+      <c r="A136" s="4"/>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="5"/>
+      <c r="A137" s="4"/>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="5"/>
+      <c r="A138" s="4"/>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="5"/>
+      <c r="A139" s="4"/>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0"/>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="5"/>
+      <c r="A141" s="4"/>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="5"/>
+      <c r="A142" s="4"/>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="5"/>
+      <c r="A143" s="4"/>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0"/>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="5"/>
+      <c r="A145" s="4"/>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="5"/>
+      <c r="A146" s="4"/>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="5"/>
+      <c r="A147" s="4"/>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="5"/>
+      <c r="A148" s="4"/>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="5"/>
+      <c r="A149" s="4"/>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="5"/>
+      <c r="A150" s="4"/>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="5"/>
+      <c r="A151" s="4"/>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="5"/>
+      <c r="A152" s="4"/>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0"/>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="5"/>
+      <c r="A154" s="4"/>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="5"/>
+      <c r="A155" s="4"/>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="5"/>
+      <c r="A156" s="4"/>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="5"/>
+      <c r="A157" s="4"/>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="5"/>
+      <c r="A158" s="4"/>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="5"/>
+      <c r="A159" s="4"/>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="9"/>
+      <c r="A160" s="8"/>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="5"/>
+      <c r="A161" s="4"/>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0"/>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="5"/>
+      <c r="A163" s="4"/>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="10"/>
+      <c r="A164" s="9"/>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="5"/>
+      <c r="A165" s="4"/>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="5"/>
+      <c r="A166" s="4"/>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="5"/>
+      <c r="A167" s="4"/>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="5"/>
+      <c r="A168" s="4"/>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="5"/>
+      <c r="A169" s="4"/>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="5"/>
+      <c r="A170" s="4"/>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="5"/>
+      <c r="A171" s="4"/>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="5"/>
+      <c r="A172" s="4"/>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="5"/>
+      <c r="A173" s="4"/>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="5"/>
+      <c r="A174" s="4"/>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="5"/>
+      <c r="A175" s="4"/>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="5"/>
+      <c r="A176" s="4"/>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="5"/>
+      <c r="A177" s="4"/>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0"/>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="5"/>
+      <c r="A179" s="4"/>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="5"/>
+      <c r="A180" s="4"/>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="5"/>
+      <c r="A181" s="4"/>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="5"/>
+      <c r="A182" s="4"/>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="5"/>
+      <c r="A183" s="4"/>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="5"/>
+      <c r="A184" s="4"/>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="5"/>
+      <c r="A185" s="4"/>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="5"/>
+      <c r="A186" s="4"/>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="5"/>
+      <c r="A187" s="4"/>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="5"/>
+      <c r="A188" s="4"/>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="5"/>
+      <c r="A189" s="4"/>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0"/>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="5"/>
+      <c r="A191" s="4"/>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="5"/>
+      <c r="A192" s="4"/>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="5"/>
+      <c r="A193" s="4"/>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="5"/>
+      <c r="A194" s="4"/>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="5"/>
+      <c r="A195" s="4"/>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="5"/>
+      <c r="A196" s="4"/>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="5"/>
+      <c r="A197" s="4"/>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="5"/>
+      <c r="A198" s="4"/>
     </row>
     <row r="199" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="5"/>
+      <c r="A199" s="4"/>
     </row>
     <row r="200" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0"/>
     </row>
     <row r="201" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="5"/>
+      <c r="A201" s="4"/>
     </row>
     <row r="202" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="5"/>
+      <c r="A202" s="4"/>
     </row>
     <row r="203" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="8"/>
+      <c r="A203" s="7"/>
     </row>
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="5"/>
+      <c r="A204" s="4"/>
     </row>
     <row r="205" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="5"/>
+      <c r="A205" s="4"/>
     </row>
     <row r="206" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="5"/>
+      <c r="A206" s="4"/>
     </row>
     <row r="207" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="5"/>
+      <c r="A207" s="4"/>
     </row>
     <row r="208" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="5"/>
+      <c r="A208" s="4"/>
     </row>
     <row r="209" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="5"/>
+      <c r="A209" s="4"/>
     </row>
     <row r="210" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="5"/>
+      <c r="A210" s="4"/>
     </row>
     <row r="211" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="5"/>
+      <c r="A211" s="4"/>
     </row>
     <row r="212" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="5"/>
+      <c r="A212" s="4"/>
     </row>
     <row r="213" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A213" s="5"/>
+      <c r="A213" s="4"/>
     </row>
     <row r="214" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A214" s="5"/>
+      <c r="A214" s="4"/>
     </row>
     <row r="215" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A215" s="5"/>
+      <c r="A215" s="4"/>
     </row>
     <row r="216" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A216" s="5"/>
+      <c r="A216" s="4"/>
     </row>
     <row r="217" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A217" s="5"/>
+      <c r="A217" s="4"/>
     </row>
     <row r="218" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A218" s="5"/>
+      <c r="A218" s="4"/>
     </row>
     <row r="219" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A219" s="5"/>
+      <c r="A219" s="4"/>
     </row>
     <row r="220" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A220" s="5"/>
+      <c r="A220" s="4"/>
     </row>
     <row r="221" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0"/>
     </row>
     <row r="222" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A222" s="5"/>
+      <c r="A222" s="4"/>
     </row>
     <row r="223" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A223" s="5"/>
+      <c r="A223" s="4"/>
     </row>
     <row r="224" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A224" s="5"/>
+      <c r="A224" s="4"/>
     </row>
     <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="5"/>
+      <c r="A225" s="4"/>
     </row>
     <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="5"/>
+      <c r="A226" s="4"/>
     </row>
     <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="5"/>
+      <c r="A227" s="4"/>
     </row>
     <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="5"/>
+      <c r="A228" s="4"/>
     </row>
     <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0"/>
     </row>
     <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="5"/>
+      <c r="A230" s="4"/>
     </row>
     <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="5"/>
+      <c r="A231" s="4"/>
     </row>
     <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="5"/>
+      <c r="A232" s="4"/>
     </row>
     <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="5"/>
+      <c r="A233" s="4"/>
     </row>
     <row r="234" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="5"/>
+      <c r="A234" s="4"/>
     </row>
     <row r="235" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="5"/>
+      <c r="A235" s="4"/>
     </row>
     <row r="236" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A236" s="9"/>
+      <c r="A236" s="8"/>
     </row>
     <row r="237" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A237" s="5"/>
+      <c r="A237" s="4"/>
     </row>
     <row r="238" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A238" s="5"/>
+      <c r="A238" s="4"/>
     </row>
     <row r="239" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="5"/>
+      <c r="A239" s="4"/>
     </row>
     <row r="240" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="5"/>
+      <c r="A240" s="4"/>
     </row>
     <row r="241" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="5"/>
+      <c r="A241" s="4"/>
     </row>
     <row r="242" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="5"/>
+      <c r="A242" s="4"/>
     </row>
     <row r="243" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="5"/>
+      <c r="A243" s="4"/>
     </row>
     <row r="244" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="5"/>
+      <c r="A244" s="4"/>
     </row>
     <row r="245" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="5"/>
+      <c r="A245" s="4"/>
     </row>
     <row r="246" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A246" s="5"/>
+      <c r="A246" s="4"/>
     </row>
     <row r="247" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="5"/>
+      <c r="A247" s="4"/>
     </row>
     <row r="248" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A248" s="5"/>
+      <c r="A248" s="4"/>
     </row>
     <row r="249" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="5"/>
+      <c r="A249" s="4"/>
     </row>
     <row r="250" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="5"/>
+      <c r="A250" s="4"/>
     </row>
     <row r="251" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A251" s="5"/>
+      <c r="A251" s="4"/>
     </row>
     <row r="252" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="5"/>
+      <c r="A252" s="4"/>
     </row>
     <row r="253" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="5"/>
+      <c r="A253" s="4"/>
     </row>
     <row r="254" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="5"/>
+      <c r="A254" s="4"/>
     </row>
     <row r="255" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="5"/>
+      <c r="A255" s="4"/>
     </row>
     <row r="256" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A256" s="5"/>
+      <c r="A256" s="4"/>
     </row>
     <row r="257" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A257" s="5"/>
+      <c r="A257" s="4"/>
     </row>
     <row r="258" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A258" s="5"/>
+      <c r="A258" s="4"/>
     </row>
     <row r="259" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A259" s="5"/>
+      <c r="A259" s="4"/>
     </row>
     <row r="260" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A260" s="9"/>
+      <c r="A260" s="8"/>
     </row>
     <row r="261" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A261" s="5"/>
+      <c r="A261" s="4"/>
     </row>
     <row r="262" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A262" s="5"/>
+      <c r="A262" s="4"/>
     </row>
     <row r="263" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A263" s="5"/>
+      <c r="A263" s="4"/>
     </row>
     <row r="264" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A264" s="5"/>
+      <c r="A264" s="4"/>
     </row>
     <row r="265" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="5"/>
+      <c r="A265" s="4"/>
     </row>
     <row r="266" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="5"/>
+      <c r="A266" s="4"/>
     </row>
     <row r="267" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A267" s="5"/>
+      <c r="A267" s="4"/>
     </row>
     <row r="268" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="7"/>
+      <c r="A268" s="6"/>
     </row>
     <row r="269" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A269" s="7"/>
+      <c r="A269" s="6"/>
     </row>
     <row r="270" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A270" s="7"/>
+      <c r="A270" s="6"/>
     </row>
     <row r="271" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A271" s="7"/>
+      <c r="A271" s="6"/>
     </row>
     <row r="272" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="7"/>
+      <c r="A272" s="6"/>
     </row>
     <row r="273" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="7"/>
+      <c r="A273" s="6"/>
     </row>
     <row r="274" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="7"/>
+      <c r="A274" s="6"/>
     </row>
     <row r="275" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="7"/>
+      <c r="A275" s="6"/>
     </row>
     <row r="276" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="7"/>
+      <c r="A276" s="6"/>
     </row>
     <row r="277" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="7"/>
+      <c r="A277" s="6"/>
     </row>
     <row r="278" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="7"/>
+      <c r="A278" s="6"/>
     </row>
     <row r="279" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A279" s="11"/>
+      <c r="A279" s="10"/>
     </row>
     <row r="280" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A280" s="7"/>
+      <c r="A280" s="6"/>
     </row>
     <row r="281" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A281" s="7"/>
+      <c r="A281" s="6"/>
     </row>
     <row r="282" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A282" s="11"/>
+      <c r="A282" s="10"/>
     </row>
     <row r="283" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A283" s="7"/>
+      <c r="A283" s="6"/>
     </row>
     <row r="284" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="7"/>
+      <c r="A284" s="6"/>
     </row>
     <row r="285" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A285" s="7"/>
+      <c r="A285" s="6"/>
     </row>
     <row r="286" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A286" s="7"/>
+      <c r="A286" s="6"/>
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="7"/>
+      <c r="A287" s="6"/>
     </row>
     <row r="288" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A288" s="7"/>
+      <c r="A288" s="6"/>
     </row>
     <row r="289" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="7"/>
+      <c r="A289" s="6"/>
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A290" s="7"/>
+      <c r="A290" s="6"/>
     </row>
     <row r="291" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A291" s="7"/>
+      <c r="A291" s="6"/>
     </row>
     <row r="292" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="11"/>
+      <c r="A292" s="10"/>
     </row>
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A293" s="7"/>
+      <c r="A293" s="6"/>
     </row>
     <row r="294" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A294" s="7"/>
+      <c r="A294" s="6"/>
     </row>
     <row r="295" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="0"/>
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A296" s="5"/>
+      <c r="A296" s="4"/>
     </row>
     <row r="297" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A297" s="5"/>
+      <c r="A297" s="4"/>
     </row>
     <row r="298" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A298" s="5"/>
+      <c r="A298" s="4"/>
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A299" s="5"/>
+      <c r="A299" s="4"/>
     </row>
     <row r="300" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A300" s="5"/>
+      <c r="A300" s="4"/>
     </row>
     <row r="301" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A301" s="5"/>
+      <c r="A301" s="4"/>
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A302" s="5"/>
+      <c r="A302" s="4"/>
     </row>
     <row r="303" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A303" s="5"/>
+      <c r="A303" s="4"/>
     </row>
     <row r="304" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A304" s="5"/>
+      <c r="A304" s="4"/>
     </row>
     <row r="305" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A305" s="5"/>
+      <c r="A305" s="4"/>
     </row>
     <row r="306" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A306" s="5"/>
+      <c r="A306" s="4"/>
     </row>
     <row r="307" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A307" s="0"/>
     </row>
     <row r="308" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A308" s="5"/>
+      <c r="A308" s="4"/>
     </row>
     <row r="309" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A309" s="9"/>
+      <c r="A309" s="8"/>
     </row>
     <row r="310" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A310" s="5"/>
+      <c r="A310" s="4"/>
     </row>
     <row r="311" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A311" s="5"/>
+      <c r="A311" s="4"/>
     </row>
     <row r="312" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A312" s="5"/>
+      <c r="A312" s="4"/>
     </row>
     <row r="313" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A313" s="5"/>
+      <c r="A313" s="4"/>
     </row>
     <row r="314" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A314" s="5"/>
+      <c r="A314" s="4"/>
     </row>
     <row r="315" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A315" s="0"/>
     </row>
     <row r="316" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A316" s="5"/>
+      <c r="A316" s="4"/>
     </row>
     <row r="317" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A317" s="5"/>
+      <c r="A317" s="4"/>
     </row>
     <row r="318" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A318" s="5"/>
+      <c r="A318" s="4"/>
     </row>
     <row r="319" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A319" s="5"/>
+      <c r="A319" s="4"/>
     </row>
     <row r="320" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A320" s="5"/>
+      <c r="A320" s="4"/>
     </row>
     <row r="321" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A321" s="5"/>
+      <c r="A321" s="4"/>
     </row>
     <row r="322" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A322" s="5"/>
+      <c r="A322" s="4"/>
     </row>
     <row r="323" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A323" s="0"/>
     </row>
     <row r="324" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A324" s="9"/>
+      <c r="A324" s="8"/>
     </row>
     <row r="325" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A325" s="9"/>
+      <c r="A325" s="8"/>
     </row>
     <row r="326" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A326" s="9"/>
+      <c r="A326" s="8"/>
     </row>
     <row r="327" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A327" s="9"/>
+      <c r="A327" s="8"/>
     </row>
     <row r="328" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A328" s="9"/>
+      <c r="A328" s="8"/>
     </row>
     <row r="329" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A329" s="9"/>
+      <c r="A329" s="8"/>
     </row>
     <row r="330" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A330" s="9"/>
+      <c r="A330" s="8"/>
     </row>
     <row r="331" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A331" s="9"/>
+      <c r="A331" s="8"/>
     </row>
     <row r="332" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A332" s="9"/>
+      <c r="A332" s="8"/>
     </row>
     <row r="333" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A333" s="9"/>
+      <c r="A333" s="8"/>
     </row>
     <row r="334" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A334" s="0"/>
     </row>
     <row r="335" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A335" s="5"/>
+      <c r="A335" s="4"/>
     </row>
     <row r="336" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A336" s="5"/>
+      <c r="A336" s="4"/>
     </row>
     <row r="337" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A337" s="5"/>
+      <c r="A337" s="4"/>
     </row>
     <row r="338" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A338" s="5"/>
+      <c r="A338" s="4"/>
     </row>
     <row r="339" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A339" s="9"/>
+      <c r="A339" s="8"/>
     </row>
     <row r="340" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A340" s="5"/>
+      <c r="A340" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>